<commit_message>
Added initial solution based on Nikolay Kostov's ASP.Net Core template
</commit_message>
<xml_diff>
--- a/Project Idea Draft - Entities and Project Description.xlsx
+++ b/Project Idea Draft - Entities and Project Description.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Description" sheetId="2" r:id="rId1"/>
     <sheet name="Entities" sheetId="1" r:id="rId2"/>
+    <sheet name="Views" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -643,7 +644,7 @@
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
@@ -895,4 +896,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added bootstrap theme - Serenity - to project. Credits added in footer. Adjusted font from 13px to 14px.
</commit_message>
<xml_diff>
--- a/Project Idea Draft - Entities and Project Description.xlsx
+++ b/Project Idea Draft - Entities and Project Description.xlsx
@@ -9,13 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Project Description" sheetId="2" r:id="rId1"/>
     <sheet name="Entities" sheetId="1" r:id="rId2"/>
     <sheet name="Views" sheetId="3" r:id="rId3"/>
+    <sheet name="Styles" sheetId="7" r:id="rId4"/>
+    <sheet name="Scripts" sheetId="6" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="test2" localSheetId="4">Scripts!$A$23:$A$36</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,8 +30,20 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="test2" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\StefanLB\Desktop\test2.txt" tab="0">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="119">
   <si>
     <t>User - Trainer</t>
   </si>
@@ -61,6 +78,9 @@
     <t>Certificate</t>
   </si>
   <si>
+    <t>Achievements</t>
+  </si>
+  <si>
     <t>Bookings (list of Booking)</t>
   </si>
   <si>
@@ -212,6 +232,174 @@
   </si>
   <si>
     <t>Last Achieved On (dateTime - most recent time achievement was reached)</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Workouts</t>
+  </si>
+  <si>
+    <t>Bookings</t>
+  </si>
+  <si>
+    <t>Create Workout</t>
+  </si>
+  <si>
+    <t>Workouts/Details</t>
+  </si>
+  <si>
+    <t>Bookings/Details</t>
+  </si>
+  <si>
+    <t>Certificates</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/css/sequence.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/css/flexslider.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/css/prettyPhoto.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/color/default.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/css/style.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/js/google-code-prettify/prettify.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/css/docs.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/css/bootstrap-responsive.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="assets/css/bootstrap.css" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;link href="https://fonts.googleapis.com/css?family=Open+Sans:400italic,400,600,700" rel="stylesheet"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/custom.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;!-- Template Custom JavaScript File --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/hover/setting.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/hover/jquery-hover-effect.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/jquery.flexslider.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/application.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/portfolio/setting.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/portfolio/jquery.quicksand.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/jquery.prettyPhoto.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/sequence/setting.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/sequence/sequence.jquery-min.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/jquery.elastislide.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/bootstrap.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/modernizr.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/google-code-prettify/prettify.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/jquery.easing.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;script src="assets/js/jquery.min.js"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;!-- JavaScript Library Files --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;!-- styles --&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;environment names="Development"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;link href="~/lib/bootstrap/dist/css/bootstrap.css" rel="stylesheet" asp-append-version="true" /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;link href="~/css/site.css" rel="stylesheet" asp-append-version="true" /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;/environment&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;environment names="Staging,Production"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;link href="~/lib/bootstrap/dist/css/bootstrap.min.css" rel="stylesheet" asp-append-version="true" /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;link href="~/css/site.min.css" rel="stylesheet" asp-append-version="true" /&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/lib/jquery/dist/jquery.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/lib/jquery-validation/dist/jquery.validate.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/lib/jquery-validation-unobtrusive/dist/jquery.validate.unobtrusive.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/lib/bootstrap/dist/js/bootstrap.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/js/site.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/lib/jquery/dist/jquery.min.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/lib/jquery-validation/dist/jquery.validate.min.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/lib/bootstrap/dist/js/bootstrap.min.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        &lt;script src="~/js/site.min.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
   </si>
 </sst>
 </file>
@@ -261,16 +449,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -281,6 +481,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="test2" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -559,77 +763,77 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -671,13 +875,13 @@
         <v>10</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -714,19 +918,19 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -737,19 +941,19 @@
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="S4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -760,19 +964,19 @@
         <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="P5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="U5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -783,16 +987,16 @@
         <v>8</v>
       </c>
       <c r="J6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="S6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -803,41 +1007,41 @@
         <v>9</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -847,49 +1051,49 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -900,12 +1104,369 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A11">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="81.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Consolidated users into Application User (Removed Coach, Trainee and contracts), updated xlsx file with view names
</commit_message>
<xml_diff>
--- a/Project Idea Draft - Entities and Project Description.xlsx
+++ b/Project Idea Draft - Entities and Project Description.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" tabRatio="688" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Description" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="127">
   <si>
     <t>User - Trainer</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Issued By (string)</t>
   </si>
   <si>
-    <t>Expiration date (dateTime?)</t>
-  </si>
-  <si>
     <t>Issued On (dateTime)</t>
   </si>
   <si>
@@ -249,9 +246,6 @@
     <t>Bookings</t>
   </si>
   <si>
-    <t>Create Workout</t>
-  </si>
-  <si>
     <t>Workouts/Details</t>
   </si>
   <si>
@@ -400,6 +394,36 @@
   </si>
   <si>
     <t xml:space="preserve">        &lt;script src="~/js/site.min.js" asp-append-version="true"&gt;&lt;/script&gt;</t>
+  </si>
+  <si>
+    <t>Expires On (dateTime?)</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>Workouts/Create</t>
+  </si>
+  <si>
+    <t>Workouts/MyWorkouts</t>
+  </si>
+  <si>
+    <t>Bookings/Create</t>
+  </si>
+  <si>
+    <t>Certificates/Add</t>
+  </si>
+  <si>
+    <t>User/?id=</t>
+  </si>
+  <si>
+    <t>Workouts/Delete</t>
+  </si>
+  <si>
+    <t>A user should be able to cancel a booking up to 30 mins before the workout</t>
   </si>
 </sst>
 </file>
@@ -449,12 +473,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,84 +781,84 @@
   <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -849,7 +874,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,13 +900,13 @@
         <v>10</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -921,16 +946,16 @@
         <v>23</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -947,13 +972,13 @@
         <v>28</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -967,16 +992,16 @@
         <v>20</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -990,10 +1015,10 @@
         <v>19</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S6" t="s">
         <v>27</v>
@@ -1010,7 +1035,7 @@
         <v>26</v>
       </c>
       <c r="M7" t="s">
-        <v>29</v>
+        <v>117</v>
       </c>
       <c r="P7" t="s">
         <v>24</v>
@@ -1041,7 +1066,7 @@
         <v>25</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
@@ -1088,12 +1113,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1104,76 +1129,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>73</v>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1181,105 +1245,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="95.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>83</v>
+      <c r="A2" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>82</v>
+      <c r="A3" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1287,6 +1352,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1294,8 +1360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,82 +1371,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>100</v>
+      <c r="A2" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>96</v>
+      <c r="A6" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
@@ -1388,85 +1454,86 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Partially Implemented Booking Controller/View/Service. "Currently Signed Up" to be fixed
</commit_message>
<xml_diff>
--- a/Project Idea Draft - Entities and Project Description.xlsx
+++ b/Project Idea Draft - Entities and Project Description.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" tabRatio="688" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9030" tabRatio="688" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Description" sheetId="2" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <definedName name="test2" localSheetId="4">Scripts!$A$23:$A$36</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -873,8 +874,8 @@
   </sheetPr>
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>